<commit_message>
Fix Viral Result test to use Tube IDs instead of generated Specimen IDs
CVDLS-209
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/viral-results-with-ct-amp-score.xlsx
+++ b/tests/ExcelImport/workbooks/viral-results-with-ct-amp-score.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BFB365-7986-744B-A749-45C8BC159E96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7101A3D-D5A2-934B-A4CA-6AC708FC2689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5280" yWindow="540" windowWidth="22020" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -97,19 +97,19 @@
     <t>D6</t>
   </si>
   <si>
-    <t>SpecimenQPCRResults1</t>
-  </si>
-  <si>
-    <t>SpecimenQPCRResults2</t>
-  </si>
-  <si>
-    <t>SpecimenQPCRResults3</t>
-  </si>
-  <si>
-    <t>SpecimenQPCRResults4</t>
-  </si>
-  <si>
     <t>QPCRResults</t>
+  </si>
+  <si>
+    <t>TubeQPCRResults0001</t>
+  </si>
+  <si>
+    <t>TubeQPCRResults0002</t>
+  </si>
+  <si>
+    <t>TubeQPCRResults0003</t>
+  </si>
+  <si>
+    <t>TubeQPCRResults0004</t>
   </si>
 </sst>
 </file>
@@ -967,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1029,7 +1029,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>19</v>
@@ -1041,7 +1041,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>20</v>
@@ -1082,7 +1082,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -1111,7 +1111,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>21</v>
@@ -1123,7 +1123,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -1152,7 +1152,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
@@ -1164,7 +1164,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
CVDLS-211 Allow specimen qpcr results without a well. viral-results-with-ct-amp-score.xlsx now has half of the results without plates or wells. Also fixed the viral-results-with-ct-amp-score.xlsx test spreadsheet since it was still referencing generated specimen accession IDs.
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/viral-results-with-ct-amp-score.xlsx
+++ b/tests/ExcelImport/workbooks/viral-results-with-ct-amp-score.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abk/Projects/covid/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7101A3D-D5A2-934B-A4CA-6AC708FC2689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F998C731-F490-5A4C-A130-78E42D448844}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="540" windowWidth="22020" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5280" yWindow="540" windowWidth="33860" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PVE690RLR_ra_calls" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>Specimen ID</t>
   </si>
@@ -88,13 +88,7 @@
     <t>Non-Negative</t>
   </si>
   <si>
-    <t>E7</t>
-  </si>
-  <si>
     <t>C5</t>
-  </si>
-  <si>
-    <t>D6</t>
   </si>
   <si>
     <t>QPCRResults</t>
@@ -968,7 +962,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -976,7 +970,7 @@
     <col min="1" max="1" width="18.1640625" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" customWidth="1"/>
     <col min="7" max="7" width="13.5" customWidth="1"/>
@@ -1029,7 +1023,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>19</v>
@@ -1041,7 +1035,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -1070,19 +1064,19 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -1111,20 +1105,16 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="C4" s="3"/>
       <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="E4" s="3"/>
       <c r="F4" t="s">
         <v>10</v>
       </c>
@@ -1152,20 +1142,16 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="C5" s="3"/>
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="E5" s="3"/>
       <c r="F5" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Import Viral Results allows Column A (Specimen ID) to contain Specimen.accessionId or Tube.accessionId
CVDLS-210
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/viral-results-with-ct-amp-score.xlsx
+++ b/tests/ExcelImport/workbooks/viral-results-with-ct-amp-score.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abk/Projects/covid/tests/ExcelImport/workbooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F998C731-F490-5A4C-A130-78E42D448844}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5E139C-914A-5A4C-A74E-CB628113A575}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="540" windowWidth="33860" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PVE690RLR_ra_calls" sheetId="1" r:id="rId1"/>
@@ -962,7 +962,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Import Viral Results verifies Well Plate Barcode and Position given when providing the other
CVDLS-201
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/viral-results-with-ct-amp-score.xlsx
+++ b/tests/ExcelImport/workbooks/viral-results-with-ct-amp-score.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD4F763-2710-ED43-932D-5D1DA5EEA036}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9696B9E1-8591-BF48-AA3F-833D42C42EAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3760" yWindow="460" windowWidth="25040" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
   <si>
     <t>Specimen ID</t>
   </si>
@@ -104,13 +104,31 @@
   </si>
   <si>
     <t>TubeQPCRResults0004</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>TubeQPCRResults0005</t>
+  </si>
+  <si>
+    <t>TubeQPCRResults0006</t>
+  </si>
+  <si>
+    <t>TubeQPCRResults0007</t>
+  </si>
+  <si>
+    <t>H10</t>
+  </si>
+  <si>
+    <t>F8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,8 +269,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,6 +462,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -599,11 +632,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -959,10 +997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -980,61 +1018,61 @@
     <col min="13" max="13" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F2" t="s">
@@ -1043,137 +1081,296 @@
       <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="2">
         <v>20.439682831841399</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="2">
         <v>0</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="2">
         <v>0</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="2">
         <v>2.05910575758501</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="3">
-        <v>100</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="3">
-        <v>18.893144729852999</v>
-      </c>
-      <c r="K3" s="3">
-        <v>1.9876543209999999</v>
-      </c>
-      <c r="L3" s="3">
-        <v>300</v>
-      </c>
-      <c r="M3" s="3">
-        <v>1.73836317116205</v>
-      </c>
+    <row r="3" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="F4" t="s">
         <v>10</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="6">
+        <v>100</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="3">
-        <v>200</v>
-      </c>
-      <c r="J4" s="3">
-        <v>19.621005213173301</v>
-      </c>
-      <c r="K4" s="3">
-        <v>400</v>
-      </c>
-      <c r="L4" s="3">
-        <v>0</v>
-      </c>
-      <c r="M4" s="3">
-        <v>1.9685408462937799</v>
+      <c r="J4" s="6">
+        <v>18.893144729852999</v>
+      </c>
+      <c r="K4" s="6">
+        <v>1.9876543209999999</v>
+      </c>
+      <c r="L4" s="6">
+        <v>300</v>
+      </c>
+      <c r="M4" s="6">
+        <v>1.73836317116205</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3"/>
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="F5" t="s">
         <v>10</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2">
+        <v>100</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="3">
+      <c r="J5" s="2">
+        <v>18.893144729852999</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1.9876543209999999</v>
+      </c>
+      <c r="L5" s="2">
+        <v>300</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1.73836317116205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="2">
+        <v>200</v>
+      </c>
+      <c r="J6" s="2">
+        <v>19.621005213173301</v>
+      </c>
+      <c r="K6" s="2">
+        <v>400</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1.9685408462937799</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="2">
         <v>500</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J7" s="2">
         <v>21.987654320000001</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K7" s="2">
         <v>0</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L7" s="2">
         <v>600</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="6">
+        <v>500</v>
+      </c>
+      <c r="J8" s="6">
+        <v>21.987654320000001</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0</v>
+      </c>
+      <c r="L8" s="6">
+        <v>600</v>
+      </c>
+      <c r="M8" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="6">
+        <v>500</v>
+      </c>
+      <c r="J9" s="6">
+        <v>21.987654320000001</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0</v>
+      </c>
+      <c r="L9" s="6">
+        <v>600</v>
+      </c>
+      <c r="M9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="6">
+        <v>500</v>
+      </c>
+      <c r="J10" s="6">
+        <v>21.987654320000001</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
+      <c r="L10" s="6">
+        <v>600</v>
+      </c>
+      <c r="M10" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CVDLS-205 Add tests for auto-creating missing plates and wells during qpcr results import
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/viral-results-with-ct-amp-score.xlsx
+++ b/tests/ExcelImport/workbooks/viral-results-with-ct-amp-score.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abk/Projects/covid/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD4F763-2710-ED43-932D-5D1DA5EEA036}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC35AAE2-1C51-0242-8F4E-879BF918CE16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3760" yWindow="460" windowWidth="25040" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>Specimen ID</t>
   </si>
@@ -104,6 +104,18 @@
   </si>
   <si>
     <t>TubeQPCRResults0004</t>
+  </si>
+  <si>
+    <t>TubeQPCRResults0005</t>
+  </si>
+  <si>
+    <t>TubeQPCRResults0006</t>
+  </si>
+  <si>
+    <t>UnknownPlate</t>
+  </si>
+  <si>
+    <t>A2</t>
   </si>
 </sst>
 </file>
@@ -959,10 +971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1177,6 +1189,88 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="3">
+        <v>200</v>
+      </c>
+      <c r="J6" s="3">
+        <v>19.621005213173301</v>
+      </c>
+      <c r="K6" s="3">
+        <v>400</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="M6" s="3">
+        <v>1.9685408462937799</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="3">
+        <v>500</v>
+      </c>
+      <c r="J7" s="3">
+        <v>21.987654320000001</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <v>600</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Viral Results now use terms Detected, Not Detected, Inconclusive
New terms replace Positive, Negative, Non-Negative respectively.
Recommended is still a valid conclusion but should not be used moving forward.

Excel upload of Viral Results must use the new terms.
Old results in production will also use these new terms.

CVDLS-276
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/viral-results-with-ct-amp-score.xlsx
+++ b/tests/ExcelImport/workbooks/viral-results-with-ct-amp-score.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82023F1B-7A16-F14C-BFF5-963CF0B10837}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60679B4-BA30-CC4E-A58B-6336FB8E3D08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3760" yWindow="460" windowWidth="25040" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,9 +40,6 @@
     <t>Storage Location</t>
   </si>
   <si>
-    <t>Negative</t>
-  </si>
-  <si>
     <t>A1</t>
   </si>
   <si>
@@ -76,15 +73,9 @@
     <t>Undetermined</t>
   </si>
   <si>
-    <t>Positive</t>
-  </si>
-  <si>
     <t>Recommended</t>
   </si>
   <si>
-    <t>Non-Negative</t>
-  </si>
-  <si>
     <t>C5</t>
   </si>
   <si>
@@ -167,6 +158,15 @@
   </si>
   <si>
     <t>SpecimenId0005</t>
+  </si>
+  <si>
+    <t>Detected</t>
+  </si>
+  <si>
+    <t>Inconclusive</t>
+  </si>
+  <si>
+    <t>Not Detected</t>
   </si>
 </sst>
 </file>
@@ -1045,7 +1045,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1074,7 +1074,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -1086,51 +1086,51 @@
         <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J2" s="2">
         <v>20.439682831841399</v>
@@ -1151,28 +1151,28 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
         <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
       </c>
       <c r="H4" s="6">
         <v>100</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J4" s="6">
         <v>18.893144729852999</v>
@@ -1189,31 +1189,31 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
       </c>
       <c r="H5" s="2">
         <v>100</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J5" s="2">
         <v>18.893144729852999</v>
@@ -1230,28 +1230,28 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" t="s">
-        <v>10</v>
-      </c>
       <c r="H6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I6" s="2">
         <v>200</v>
@@ -1271,28 +1271,28 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" t="s">
         <v>9</v>
       </c>
-      <c r="G7" t="s">
-        <v>10</v>
-      </c>
       <c r="H7" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I7" s="6">
         <v>500</v>
@@ -1312,28 +1312,28 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
         <v>9</v>
       </c>
-      <c r="G8" t="s">
-        <v>10</v>
-      </c>
       <c r="H8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I8" s="2">
         <v>500</v>
@@ -1353,28 +1353,28 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
         <v>9</v>
       </c>
-      <c r="G9" t="s">
-        <v>10</v>
-      </c>
       <c r="H9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I9" s="2">
         <v>500</v>
@@ -1394,26 +1394,26 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
         <v>9</v>
       </c>
-      <c r="G10" t="s">
-        <v>10</v>
-      </c>
       <c r="H10" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I10" s="6">
         <v>500</v>
@@ -1433,26 +1433,26 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" t="s">
         <v>9</v>
       </c>
-      <c r="G11" t="s">
-        <v>10</v>
-      </c>
       <c r="H11" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I11" s="6">
         <v>500</v>
@@ -1472,26 +1472,26 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" t="s">
         <v>9</v>
       </c>
-      <c r="G12" t="s">
-        <v>10</v>
-      </c>
       <c r="H12" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I12" s="6">
         <v>500</v>
@@ -1511,28 +1511,28 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" t="s">
         <v>9</v>
       </c>
-      <c r="G13" t="s">
-        <v>10</v>
-      </c>
       <c r="H13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I13" s="2">
         <v>500</v>

</xml_diff>